<commit_message>
create medication & medicationstat table,model&seed
</commit_message>
<xml_diff>
--- a/db/seed-lookup.xlsx
+++ b/db/seed-lookup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" firstSheet="24" activeTab="33"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" firstSheet="23" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="2" r:id="rId1"/>
@@ -46,6 +46,7 @@
     <sheet name="Gstcode" sheetId="34" r:id="rId32"/>
     <sheet name="Documentstat" sheetId="35" r:id="rId33"/>
     <sheet name="Icdtype" sheetId="36" r:id="rId34"/>
+    <sheet name="Medicationstat" sheetId="37" r:id="rId35"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="991">
   <si>
     <t>CC</t>
   </si>
@@ -4576,6 +4577,12 @@
   </si>
   <si>
     <t>ICD10 Procedure Coding System</t>
+  </si>
+  <si>
+    <t>Given</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -13709,8 +13716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13758,6 +13765,66 @@
       <c r="D3" t="str">
         <f t="shared" si="0"/>
         <v>Icdtype.create( id: 3, code: 'ICD10-PCS', name: 'ICD10 Procedure Coding System', disabled: false)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("Medicationstat.create( id: ",A1,", code: '",B1,"', name: '",C1,"', disabled: false)")</f>
+        <v>Medicationstat.create( id: 1, code: 'O', name: 'Order', disabled: false)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>990</v>
+      </c>
+      <c r="C2" t="s">
+        <v>989</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D3" si="0">CONCATENATE("Medicationstat.create( id: ",A2,", code: '",B2,"', name: '",C2,"', disabled: false)")</f>
+        <v>Medicationstat.create( id: 2, code: 'G', name: 'Given', disabled: false)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>Medicationstat.create( id: 3, code: 'C', name: 'Cancelled', disabled: false)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add audit type seed
</commit_message>
<xml_diff>
--- a/db/seed-lookup.xlsx
+++ b/db/seed-lookup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" firstSheet="23" activeTab="34"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" firstSheet="24" activeTab="35"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="2" r:id="rId1"/>
@@ -47,6 +47,7 @@
     <sheet name="Documentstat" sheetId="35" r:id="rId33"/>
     <sheet name="Icdtype" sheetId="36" r:id="rId34"/>
     <sheet name="Medicationstat" sheetId="37" r:id="rId35"/>
+    <sheet name="Audittype" sheetId="38" r:id="rId36"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="995">
   <si>
     <t>CC</t>
   </si>
@@ -4583,6 +4584,18 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>AUTH</t>
+  </si>
+  <si>
+    <t>Authentication Audit</t>
+  </si>
+  <si>
+    <t>GENERAL</t>
+  </si>
+  <si>
+    <t>General Audit</t>
   </si>
 </sst>
 </file>
@@ -13776,7 +13789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -13825,6 +13838,54 @@
       <c r="D3" t="str">
         <f t="shared" si="0"/>
         <v>Medicationstat.create( id: 3, code: 'C', name: 'Cancelled', disabled: false)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>991</v>
+      </c>
+      <c r="C1" t="s">
+        <v>992</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("Audittype.create( id: ",A1,", code: '",B1,"', name: '",C1,"', disabled: false)")</f>
+        <v>Audittype.create( id: 1, code: 'AUTH', name: 'Authentication Audit', disabled: false)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>993</v>
+      </c>
+      <c r="C2" t="s">
+        <v>994</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2" si="0">CONCATENATE("Audittype.create( id: ",A2,", code: '",B2,"', name: '",C2,"', disabled: false)")</f>
+        <v>Audittype.create( id: 2, code: 'GENERAL', name: 'General Audit', disabled: false)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add appointmentstat, appointment & runningnumber table
</commit_message>
<xml_diff>
--- a/db/seed-lookup.xlsx
+++ b/db/seed-lookup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" firstSheet="24" activeTab="35"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" firstSheet="26" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="2" r:id="rId1"/>
@@ -48,6 +48,8 @@
     <sheet name="Icdtype" sheetId="36" r:id="rId34"/>
     <sheet name="Medicationstat" sheetId="37" r:id="rId35"/>
     <sheet name="Audittype" sheetId="38" r:id="rId36"/>
+    <sheet name="Appointmentstat" sheetId="39" r:id="rId37"/>
+    <sheet name="Runningnumber" sheetId="40" r:id="rId38"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="995">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="1003">
   <si>
     <t>CC</t>
   </si>
@@ -4596,6 +4598,30 @@
   </si>
   <si>
     <t>General Audit</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>Medical Record Number</t>
+  </si>
+  <si>
+    <t>Visit Number</t>
+  </si>
+  <si>
+    <t>BILL</t>
+  </si>
+  <si>
+    <t>Billing Number</t>
+  </si>
+  <si>
+    <t>PAY</t>
+  </si>
+  <si>
+    <t>Payment Number</t>
   </si>
 </sst>
 </file>
@@ -13849,7 +13875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
@@ -13886,6 +13912,132 @@
       <c r="D2" t="str">
         <f t="shared" ref="D2" si="0">CONCATENATE("Audittype.create( id: ",A2,", code: '",B2,"', name: '",C2,"', disabled: false)")</f>
         <v>Audittype.create( id: 2, code: 'GENERAL', name: 'General Audit', disabled: false)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("Appointmentstat.create( id: ",A1,", code: '",B1,"', name: '",C1,"', disabled: false)")</f>
+        <v>Appointmentstat.create( id: 1, code: 'N', name: 'New', disabled: false)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE("Appointmentstat.create( id: ",A2,", code: '",B2,"', name: '",C2,"', disabled: false)")</f>
+        <v>Appointmentstat.create( id: 2, code: 'C', name: 'Cancelled', disabled: false)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>996</v>
+      </c>
+      <c r="C1" t="s">
+        <v>997</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("Runningnumber.create( id: ",A1,", code: '",B1,"', name: '",C1,"', running: 1)")</f>
+        <v>Runningnumber.create( id: 1, code: 'RN', name: 'Medical Record Number', running: 1)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>995</v>
+      </c>
+      <c r="C2" t="s">
+        <v>998</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D4" si="0">CONCATENATE("Runningnumber.create( id: ",A2,", code: '",B2,"', name: '",C2,"', running: 1)")</f>
+        <v>Runningnumber.create( id: 2, code: 'SN', name: 'Visit Number', running: 1)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>999</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>Runningnumber.create( id: 3, code: 'BILL', name: 'Billing Number', running: 1)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Runningnumber.create( id: 4, code: 'PAY', name: 'Payment Number', running: 1)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>